<commit_message>
found another missing data item
</commit_message>
<xml_diff>
--- a/dataitems.xlsx
+++ b/dataitems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repository\cimir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{974CE062-4E87-430E-97F0-65D55777A079}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FB3B9EFF-6CED-41C1-A34F-7BC85E75FFAE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" xr2:uid="{3CF03427-5C64-4814-8BC6-67AF8F3202AA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>day-air-tmp-max</t>
+  </si>
+  <si>
+    <t>Minimum Vapor Pressure</t>
+  </si>
+  <si>
+    <t>day-vap-pres-min</t>
   </si>
 </sst>
 </file>
@@ -637,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5BE83A-586A-4C19-8B00-5DCA826D1DBF}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,10 +897,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -905,10 +911,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -919,10 +925,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
@@ -933,10 +939,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -947,10 +953,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -961,10 +967,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
@@ -975,10 +981,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -989,10 +995,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -1003,10 +1009,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -1017,10 +1023,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -1031,10 +1037,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -1045,10 +1051,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -1059,13 +1065,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -1073,10 +1079,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
         <v>61</v>
@@ -1087,10 +1093,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
         <v>61</v>
@@ -1101,10 +1107,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
         <v>61</v>
@@ -1115,10 +1121,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
         <v>61</v>
@@ -1129,10 +1135,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
         <v>61</v>
@@ -1143,10 +1149,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
         <v>61</v>
@@ -1157,10 +1163,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
         <v>61</v>
@@ -1171,10 +1177,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
@@ -1185,10 +1191,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C39" t="s">
         <v>61</v>
@@ -1199,10 +1205,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C40" t="s">
         <v>61</v>
@@ -1213,10 +1219,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
         <v>61</v>
@@ -1227,10 +1233,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
         <v>61</v>
@@ -1241,15 +1247,29 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>81</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>82</v>
       </c>
-      <c r="C43" t="s">
-        <v>61</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C44" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>